<commit_message>
actualizacion de cartola al 22 de julio
</commit_message>
<xml_diff>
--- a/cartola_junio_2025.xlsx
+++ b/cartola_junio_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\manager8\comunes\importacion\api_cluster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17031E1F-E1BC-4E8B-B05B-59CCF56A040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87567C0-D2C2-4861-AC6E-1450182D91B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F0B3DEB9-4C62-4D57-84BC-B1B8A40A9B47}"/>
   </bookViews>
@@ -1796,10 +1796,10 @@
   <dimension ref="A1:N332"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C181" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C187" sqref="C187"/>
+      <selection pane="bottomRight" activeCell="H183" sqref="H183:K183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
actualizo cartola hasta el 22 de julio
</commit_message>
<xml_diff>
--- a/cartola_junio_2025.xlsx
+++ b/cartola_junio_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\manager8\comunes\importacion\api_cluster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87567C0-D2C2-4861-AC6E-1450182D91B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EF09CF-26D6-4A2D-AAD5-908A1B60BC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F0B3DEB9-4C62-4D57-84BC-B1B8A40A9B47}"/>
   </bookViews>
@@ -1193,12 +1193,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1206,6 +1200,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1799,7 +1799,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H183" sqref="H183:K183"/>
+      <selection pane="bottomRight" activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2449,10 +2449,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2468,17 +2468,17 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="21" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
     </row>
     <row r="2" spans="1:14" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -10670,415 +10670,238 @@
     <filterColumn colId="9" showButton="0"/>
   </autoFilter>
   <mergeCells count="665">
-    <mergeCell ref="H325:K325"/>
-    <mergeCell ref="H326:K326"/>
-    <mergeCell ref="H327:K327"/>
-    <mergeCell ref="H328:K328"/>
-    <mergeCell ref="H329:K329"/>
-    <mergeCell ref="H330:K330"/>
-    <mergeCell ref="H331:K331"/>
-    <mergeCell ref="H332:K332"/>
-    <mergeCell ref="A332:B332"/>
-    <mergeCell ref="H303:K303"/>
-    <mergeCell ref="H304:K304"/>
-    <mergeCell ref="H305:K305"/>
-    <mergeCell ref="H306:K306"/>
-    <mergeCell ref="H307:K307"/>
-    <mergeCell ref="H308:K308"/>
-    <mergeCell ref="H309:K309"/>
-    <mergeCell ref="H310:K310"/>
-    <mergeCell ref="H311:K311"/>
-    <mergeCell ref="H312:K312"/>
-    <mergeCell ref="H313:K313"/>
-    <mergeCell ref="H314:K314"/>
-    <mergeCell ref="H315:K315"/>
-    <mergeCell ref="H316:K316"/>
-    <mergeCell ref="H317:K317"/>
-    <mergeCell ref="H318:K318"/>
-    <mergeCell ref="H319:K319"/>
-    <mergeCell ref="H320:K320"/>
-    <mergeCell ref="H321:K321"/>
-    <mergeCell ref="H322:K322"/>
-    <mergeCell ref="H323:K323"/>
-    <mergeCell ref="H324:K324"/>
-    <mergeCell ref="A327:B327"/>
-    <mergeCell ref="A328:B328"/>
-    <mergeCell ref="A329:B329"/>
-    <mergeCell ref="A330:B330"/>
-    <mergeCell ref="A331:B331"/>
-    <mergeCell ref="A322:B322"/>
-    <mergeCell ref="A323:B323"/>
-    <mergeCell ref="A324:B324"/>
-    <mergeCell ref="A325:B325"/>
-    <mergeCell ref="A326:B326"/>
-    <mergeCell ref="A317:B317"/>
-    <mergeCell ref="A318:B318"/>
-    <mergeCell ref="A319:B319"/>
-    <mergeCell ref="A320:B320"/>
-    <mergeCell ref="A321:B321"/>
-    <mergeCell ref="A312:B312"/>
-    <mergeCell ref="A313:B313"/>
-    <mergeCell ref="A314:B314"/>
-    <mergeCell ref="A315:B315"/>
-    <mergeCell ref="A316:B316"/>
-    <mergeCell ref="A307:B307"/>
-    <mergeCell ref="A308:B308"/>
-    <mergeCell ref="A309:B309"/>
-    <mergeCell ref="A310:B310"/>
-    <mergeCell ref="A311:B311"/>
-    <mergeCell ref="A303:B303"/>
-    <mergeCell ref="A304:B304"/>
-    <mergeCell ref="A305:B305"/>
-    <mergeCell ref="A306:B306"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="H58:K58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="H59:K59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="H57:K57"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="H61:K61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="H63:K63"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="H71:K71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="H68:K68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="H106:K106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="H130:K130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="H131:K131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="H132:K132"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="H128:K128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="H129:K129"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="H136:K136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="H133:K133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="H134:K134"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="H139:K139"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="H149:K149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="H150:K150"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="H145:K145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="H154:K154"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="H155:K155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="H156:K156"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="H151:K151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="H152:K152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="H153:K153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="H160:K160"/>
-    <mergeCell ref="A161:B161"/>
-    <mergeCell ref="H161:K161"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="H162:K162"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="H157:K157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="H158:K158"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="H159:K159"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="H166:K166"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="H167:K167"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="H168:K168"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="H163:K163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="H164:K164"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="H165:K165"/>
-    <mergeCell ref="H177:K177"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="H172:K172"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="H173:K173"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="H174:K174"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="H169:K169"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="H170:K170"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="H171:K171"/>
+    <mergeCell ref="H301:K301"/>
+    <mergeCell ref="H302:K302"/>
+    <mergeCell ref="A301:B301"/>
+    <mergeCell ref="A302:B302"/>
+    <mergeCell ref="H187:K187"/>
+    <mergeCell ref="H188:K188"/>
+    <mergeCell ref="H189:K189"/>
+    <mergeCell ref="H190:K190"/>
+    <mergeCell ref="H191:K191"/>
+    <mergeCell ref="H192:K192"/>
+    <mergeCell ref="H193:K193"/>
+    <mergeCell ref="H194:K194"/>
+    <mergeCell ref="H195:K195"/>
+    <mergeCell ref="H196:K196"/>
+    <mergeCell ref="H197:K197"/>
+    <mergeCell ref="H198:K198"/>
+    <mergeCell ref="H199:K199"/>
+    <mergeCell ref="H200:K200"/>
+    <mergeCell ref="H201:K201"/>
+    <mergeCell ref="H202:K202"/>
+    <mergeCell ref="H203:K203"/>
+    <mergeCell ref="H204:K204"/>
+    <mergeCell ref="A298:B298"/>
+    <mergeCell ref="A299:B299"/>
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="H298:K298"/>
+    <mergeCell ref="H299:K299"/>
+    <mergeCell ref="H300:K300"/>
+    <mergeCell ref="A295:B295"/>
+    <mergeCell ref="A296:B296"/>
+    <mergeCell ref="A297:B297"/>
+    <mergeCell ref="H295:K295"/>
+    <mergeCell ref="H296:K296"/>
+    <mergeCell ref="H297:K297"/>
+    <mergeCell ref="A292:B292"/>
+    <mergeCell ref="A293:B293"/>
+    <mergeCell ref="A294:B294"/>
+    <mergeCell ref="H292:K292"/>
+    <mergeCell ref="H293:K293"/>
+    <mergeCell ref="H294:K294"/>
+    <mergeCell ref="A289:B289"/>
+    <mergeCell ref="A290:B290"/>
+    <mergeCell ref="A291:B291"/>
+    <mergeCell ref="H289:K289"/>
+    <mergeCell ref="H290:K290"/>
+    <mergeCell ref="H291:K291"/>
+    <mergeCell ref="A286:B286"/>
+    <mergeCell ref="A287:B287"/>
+    <mergeCell ref="A288:B288"/>
+    <mergeCell ref="H286:K286"/>
+    <mergeCell ref="H287:K287"/>
+    <mergeCell ref="H288:K288"/>
+    <mergeCell ref="A283:B283"/>
+    <mergeCell ref="A284:B284"/>
+    <mergeCell ref="A285:B285"/>
+    <mergeCell ref="H283:K283"/>
+    <mergeCell ref="H284:K284"/>
+    <mergeCell ref="H285:K285"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="A281:B281"/>
+    <mergeCell ref="A282:B282"/>
+    <mergeCell ref="H280:K280"/>
+    <mergeCell ref="H281:K281"/>
+    <mergeCell ref="H282:K282"/>
+    <mergeCell ref="A277:B277"/>
+    <mergeCell ref="A278:B278"/>
+    <mergeCell ref="A279:B279"/>
+    <mergeCell ref="H277:K277"/>
+    <mergeCell ref="H278:K278"/>
+    <mergeCell ref="H279:K279"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A275:B275"/>
+    <mergeCell ref="A276:B276"/>
+    <mergeCell ref="H274:K274"/>
+    <mergeCell ref="H275:K275"/>
+    <mergeCell ref="H276:K276"/>
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="A272:B272"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="H271:K271"/>
+    <mergeCell ref="H272:K272"/>
+    <mergeCell ref="H273:K273"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A269:B269"/>
+    <mergeCell ref="A270:B270"/>
+    <mergeCell ref="H268:K268"/>
+    <mergeCell ref="H269:K269"/>
+    <mergeCell ref="H270:K270"/>
+    <mergeCell ref="A265:B265"/>
+    <mergeCell ref="A266:B266"/>
+    <mergeCell ref="A267:B267"/>
+    <mergeCell ref="H265:K265"/>
+    <mergeCell ref="H266:K266"/>
+    <mergeCell ref="H267:K267"/>
+    <mergeCell ref="A262:B262"/>
+    <mergeCell ref="A263:B263"/>
+    <mergeCell ref="A264:B264"/>
+    <mergeCell ref="H262:K262"/>
+    <mergeCell ref="H263:K263"/>
+    <mergeCell ref="H264:K264"/>
+    <mergeCell ref="A259:B259"/>
+    <mergeCell ref="A260:B260"/>
+    <mergeCell ref="A261:B261"/>
+    <mergeCell ref="H259:K259"/>
+    <mergeCell ref="H260:K260"/>
+    <mergeCell ref="H261:K261"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="A258:B258"/>
+    <mergeCell ref="H256:K256"/>
+    <mergeCell ref="H257:K257"/>
+    <mergeCell ref="H258:K258"/>
+    <mergeCell ref="A253:B253"/>
+    <mergeCell ref="A254:B254"/>
+    <mergeCell ref="A255:B255"/>
+    <mergeCell ref="H253:K253"/>
+    <mergeCell ref="H254:K254"/>
+    <mergeCell ref="H255:K255"/>
+    <mergeCell ref="A250:B250"/>
+    <mergeCell ref="A251:B251"/>
+    <mergeCell ref="A252:B252"/>
+    <mergeCell ref="H250:K250"/>
+    <mergeCell ref="H251:K251"/>
+    <mergeCell ref="H252:K252"/>
+    <mergeCell ref="A247:B247"/>
+    <mergeCell ref="A248:B248"/>
+    <mergeCell ref="A249:B249"/>
+    <mergeCell ref="H247:K247"/>
+    <mergeCell ref="H248:K248"/>
+    <mergeCell ref="H249:K249"/>
+    <mergeCell ref="A244:B244"/>
+    <mergeCell ref="A245:B245"/>
+    <mergeCell ref="A246:B246"/>
+    <mergeCell ref="H244:K244"/>
+    <mergeCell ref="H245:K245"/>
+    <mergeCell ref="H246:K246"/>
+    <mergeCell ref="A241:B241"/>
+    <mergeCell ref="A242:B242"/>
+    <mergeCell ref="A243:B243"/>
+    <mergeCell ref="H241:K241"/>
+    <mergeCell ref="H242:K242"/>
+    <mergeCell ref="H243:K243"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A239:B239"/>
+    <mergeCell ref="A240:B240"/>
+    <mergeCell ref="H238:K238"/>
+    <mergeCell ref="H239:K239"/>
+    <mergeCell ref="H240:K240"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="A236:B236"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="H235:K235"/>
+    <mergeCell ref="H236:K236"/>
+    <mergeCell ref="H237:K237"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A233:B233"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="H232:K232"/>
+    <mergeCell ref="H233:K233"/>
+    <mergeCell ref="H234:K234"/>
+    <mergeCell ref="A229:B229"/>
+    <mergeCell ref="A230:B230"/>
+    <mergeCell ref="A231:B231"/>
+    <mergeCell ref="H229:K229"/>
+    <mergeCell ref="H230:K230"/>
+    <mergeCell ref="H231:K231"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A227:B227"/>
+    <mergeCell ref="A228:B228"/>
+    <mergeCell ref="H226:K226"/>
+    <mergeCell ref="H227:K227"/>
+    <mergeCell ref="H228:K228"/>
+    <mergeCell ref="A223:B223"/>
+    <mergeCell ref="A224:B224"/>
+    <mergeCell ref="A225:B225"/>
+    <mergeCell ref="H223:K223"/>
+    <mergeCell ref="H224:K224"/>
+    <mergeCell ref="H225:K225"/>
+    <mergeCell ref="A220:B220"/>
+    <mergeCell ref="A221:B221"/>
+    <mergeCell ref="A222:B222"/>
+    <mergeCell ref="H220:K220"/>
+    <mergeCell ref="H221:K221"/>
+    <mergeCell ref="H222:K222"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A219:B219"/>
+    <mergeCell ref="H217:K217"/>
+    <mergeCell ref="H218:K218"/>
+    <mergeCell ref="H219:K219"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="A216:B216"/>
+    <mergeCell ref="H214:K214"/>
+    <mergeCell ref="H215:K215"/>
+    <mergeCell ref="H216:K216"/>
+    <mergeCell ref="A211:B211"/>
+    <mergeCell ref="A212:B212"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="H211:K211"/>
+    <mergeCell ref="H212:K212"/>
+    <mergeCell ref="H213:K213"/>
+    <mergeCell ref="A208:B208"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A210:B210"/>
+    <mergeCell ref="H208:K208"/>
+    <mergeCell ref="H209:K209"/>
+    <mergeCell ref="H210:K210"/>
+    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="A206:B206"/>
+    <mergeCell ref="A207:B207"/>
+    <mergeCell ref="H205:K205"/>
+    <mergeCell ref="H206:K206"/>
+    <mergeCell ref="H207:K207"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A198:B198"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A194:B194"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A189:B189"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="A184:B184"/>
     <mergeCell ref="H184:K184"/>
@@ -11103,238 +10926,415 @@
     <mergeCell ref="A176:B176"/>
     <mergeCell ref="H176:K176"/>
     <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A194:B194"/>
-    <mergeCell ref="A195:B195"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A189:B189"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A203:B203"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A199:B199"/>
-    <mergeCell ref="A200:B200"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A198:B198"/>
-    <mergeCell ref="A208:B208"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A210:B210"/>
-    <mergeCell ref="H208:K208"/>
-    <mergeCell ref="H209:K209"/>
-    <mergeCell ref="H210:K210"/>
-    <mergeCell ref="A205:B205"/>
-    <mergeCell ref="A206:B206"/>
-    <mergeCell ref="A207:B207"/>
-    <mergeCell ref="H205:K205"/>
-    <mergeCell ref="H206:K206"/>
-    <mergeCell ref="H207:K207"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A216:B216"/>
-    <mergeCell ref="H214:K214"/>
-    <mergeCell ref="H215:K215"/>
-    <mergeCell ref="H216:K216"/>
-    <mergeCell ref="A211:B211"/>
-    <mergeCell ref="A212:B212"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="H211:K211"/>
-    <mergeCell ref="H212:K212"/>
-    <mergeCell ref="H213:K213"/>
-    <mergeCell ref="A220:B220"/>
-    <mergeCell ref="A221:B221"/>
-    <mergeCell ref="A222:B222"/>
-    <mergeCell ref="H220:K220"/>
-    <mergeCell ref="H221:K221"/>
-    <mergeCell ref="H222:K222"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A219:B219"/>
-    <mergeCell ref="H217:K217"/>
-    <mergeCell ref="H218:K218"/>
-    <mergeCell ref="H219:K219"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A227:B227"/>
-    <mergeCell ref="A228:B228"/>
-    <mergeCell ref="H226:K226"/>
-    <mergeCell ref="H227:K227"/>
-    <mergeCell ref="H228:K228"/>
-    <mergeCell ref="A223:B223"/>
-    <mergeCell ref="A224:B224"/>
-    <mergeCell ref="A225:B225"/>
-    <mergeCell ref="H223:K223"/>
-    <mergeCell ref="H224:K224"/>
-    <mergeCell ref="H225:K225"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A233:B233"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="H232:K232"/>
-    <mergeCell ref="H233:K233"/>
-    <mergeCell ref="H234:K234"/>
-    <mergeCell ref="A229:B229"/>
-    <mergeCell ref="A230:B230"/>
-    <mergeCell ref="A231:B231"/>
-    <mergeCell ref="H229:K229"/>
-    <mergeCell ref="H230:K230"/>
-    <mergeCell ref="H231:K231"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="A239:B239"/>
-    <mergeCell ref="A240:B240"/>
-    <mergeCell ref="H238:K238"/>
-    <mergeCell ref="H239:K239"/>
-    <mergeCell ref="H240:K240"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="A236:B236"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="H235:K235"/>
-    <mergeCell ref="H236:K236"/>
-    <mergeCell ref="H237:K237"/>
-    <mergeCell ref="A244:B244"/>
-    <mergeCell ref="A245:B245"/>
-    <mergeCell ref="A246:B246"/>
-    <mergeCell ref="H244:K244"/>
-    <mergeCell ref="H245:K245"/>
-    <mergeCell ref="H246:K246"/>
-    <mergeCell ref="A241:B241"/>
-    <mergeCell ref="A242:B242"/>
-    <mergeCell ref="A243:B243"/>
-    <mergeCell ref="H241:K241"/>
-    <mergeCell ref="H242:K242"/>
-    <mergeCell ref="H243:K243"/>
-    <mergeCell ref="A250:B250"/>
-    <mergeCell ref="A251:B251"/>
-    <mergeCell ref="A252:B252"/>
-    <mergeCell ref="H250:K250"/>
-    <mergeCell ref="H251:K251"/>
-    <mergeCell ref="H252:K252"/>
-    <mergeCell ref="A247:B247"/>
-    <mergeCell ref="A248:B248"/>
-    <mergeCell ref="A249:B249"/>
-    <mergeCell ref="H247:K247"/>
-    <mergeCell ref="H248:K248"/>
-    <mergeCell ref="H249:K249"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="A257:B257"/>
-    <mergeCell ref="A258:B258"/>
-    <mergeCell ref="H256:K256"/>
-    <mergeCell ref="H257:K257"/>
-    <mergeCell ref="H258:K258"/>
-    <mergeCell ref="A253:B253"/>
-    <mergeCell ref="A254:B254"/>
-    <mergeCell ref="A255:B255"/>
-    <mergeCell ref="H253:K253"/>
-    <mergeCell ref="H254:K254"/>
-    <mergeCell ref="H255:K255"/>
-    <mergeCell ref="A262:B262"/>
-    <mergeCell ref="A263:B263"/>
-    <mergeCell ref="A264:B264"/>
-    <mergeCell ref="H262:K262"/>
-    <mergeCell ref="H263:K263"/>
-    <mergeCell ref="H264:K264"/>
-    <mergeCell ref="A259:B259"/>
-    <mergeCell ref="A260:B260"/>
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="H259:K259"/>
-    <mergeCell ref="H260:K260"/>
-    <mergeCell ref="H261:K261"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A269:B269"/>
-    <mergeCell ref="A270:B270"/>
-    <mergeCell ref="H268:K268"/>
-    <mergeCell ref="H269:K269"/>
-    <mergeCell ref="H270:K270"/>
-    <mergeCell ref="A265:B265"/>
-    <mergeCell ref="A266:B266"/>
-    <mergeCell ref="A267:B267"/>
-    <mergeCell ref="H265:K265"/>
-    <mergeCell ref="H266:K266"/>
-    <mergeCell ref="H267:K267"/>
-    <mergeCell ref="A274:B274"/>
-    <mergeCell ref="A275:B275"/>
-    <mergeCell ref="A276:B276"/>
-    <mergeCell ref="H274:K274"/>
-    <mergeCell ref="H275:K275"/>
-    <mergeCell ref="H276:K276"/>
-    <mergeCell ref="A271:B271"/>
-    <mergeCell ref="A272:B272"/>
-    <mergeCell ref="A273:B273"/>
-    <mergeCell ref="H271:K271"/>
-    <mergeCell ref="H272:K272"/>
-    <mergeCell ref="H273:K273"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="A281:B281"/>
-    <mergeCell ref="A282:B282"/>
-    <mergeCell ref="H280:K280"/>
-    <mergeCell ref="H281:K281"/>
-    <mergeCell ref="H282:K282"/>
-    <mergeCell ref="A277:B277"/>
-    <mergeCell ref="A278:B278"/>
-    <mergeCell ref="A279:B279"/>
-    <mergeCell ref="H277:K277"/>
-    <mergeCell ref="H278:K278"/>
-    <mergeCell ref="H279:K279"/>
-    <mergeCell ref="A286:B286"/>
-    <mergeCell ref="A287:B287"/>
-    <mergeCell ref="A288:B288"/>
-    <mergeCell ref="H286:K286"/>
-    <mergeCell ref="H287:K287"/>
-    <mergeCell ref="H288:K288"/>
-    <mergeCell ref="A283:B283"/>
-    <mergeCell ref="A284:B284"/>
-    <mergeCell ref="A285:B285"/>
-    <mergeCell ref="H283:K283"/>
-    <mergeCell ref="H284:K284"/>
-    <mergeCell ref="H285:K285"/>
-    <mergeCell ref="A292:B292"/>
-    <mergeCell ref="A293:B293"/>
-    <mergeCell ref="A294:B294"/>
-    <mergeCell ref="H292:K292"/>
-    <mergeCell ref="H293:K293"/>
-    <mergeCell ref="H294:K294"/>
-    <mergeCell ref="A289:B289"/>
-    <mergeCell ref="A290:B290"/>
-    <mergeCell ref="A291:B291"/>
-    <mergeCell ref="H289:K289"/>
-    <mergeCell ref="H290:K290"/>
-    <mergeCell ref="H291:K291"/>
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="H298:K298"/>
-    <mergeCell ref="H299:K299"/>
-    <mergeCell ref="H300:K300"/>
-    <mergeCell ref="A295:B295"/>
-    <mergeCell ref="A296:B296"/>
-    <mergeCell ref="A297:B297"/>
-    <mergeCell ref="H295:K295"/>
-    <mergeCell ref="H296:K296"/>
-    <mergeCell ref="H297:K297"/>
-    <mergeCell ref="H301:K301"/>
-    <mergeCell ref="H302:K302"/>
-    <mergeCell ref="A301:B301"/>
-    <mergeCell ref="A302:B302"/>
-    <mergeCell ref="H187:K187"/>
-    <mergeCell ref="H188:K188"/>
-    <mergeCell ref="H189:K189"/>
-    <mergeCell ref="H190:K190"/>
-    <mergeCell ref="H191:K191"/>
-    <mergeCell ref="H192:K192"/>
-    <mergeCell ref="H193:K193"/>
-    <mergeCell ref="H194:K194"/>
-    <mergeCell ref="H195:K195"/>
-    <mergeCell ref="H196:K196"/>
-    <mergeCell ref="H197:K197"/>
-    <mergeCell ref="H198:K198"/>
-    <mergeCell ref="H199:K199"/>
-    <mergeCell ref="H200:K200"/>
-    <mergeCell ref="H201:K201"/>
-    <mergeCell ref="H202:K202"/>
-    <mergeCell ref="H203:K203"/>
-    <mergeCell ref="H204:K204"/>
-    <mergeCell ref="A298:B298"/>
-    <mergeCell ref="A299:B299"/>
+    <mergeCell ref="H177:K177"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="H172:K172"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="H173:K173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="H174:K174"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="H169:K169"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="H170:K170"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="H171:K171"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="H166:K166"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="H167:K167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="H168:K168"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="H163:K163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="H164:K164"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="H165:K165"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="H160:K160"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="H161:K161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="H162:K162"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="H157:K157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="H158:K158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="H159:K159"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="H154:K154"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="H155:K155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="H156:K156"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="H151:K151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="H152:K152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="H153:K153"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="H149:K149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="H150:K150"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="H139:K139"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="H136:K136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="H134:K134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="H130:K130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="H131:K131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="H132:K132"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="H128:K128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="H121:K121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="H106:K106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="H71:K71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="H68:K68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="H61:K61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="H63:K63"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="H59:K59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="A307:B307"/>
+    <mergeCell ref="A308:B308"/>
+    <mergeCell ref="A309:B309"/>
+    <mergeCell ref="A310:B310"/>
+    <mergeCell ref="A311:B311"/>
+    <mergeCell ref="A303:B303"/>
+    <mergeCell ref="A304:B304"/>
+    <mergeCell ref="A305:B305"/>
+    <mergeCell ref="A306:B306"/>
+    <mergeCell ref="A317:B317"/>
+    <mergeCell ref="A318:B318"/>
+    <mergeCell ref="A319:B319"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="A321:B321"/>
+    <mergeCell ref="A312:B312"/>
+    <mergeCell ref="A313:B313"/>
+    <mergeCell ref="A314:B314"/>
+    <mergeCell ref="A315:B315"/>
+    <mergeCell ref="A316:B316"/>
+    <mergeCell ref="H321:K321"/>
+    <mergeCell ref="H322:K322"/>
+    <mergeCell ref="H323:K323"/>
+    <mergeCell ref="H324:K324"/>
+    <mergeCell ref="A327:B327"/>
+    <mergeCell ref="A328:B328"/>
+    <mergeCell ref="A329:B329"/>
+    <mergeCell ref="A330:B330"/>
+    <mergeCell ref="A331:B331"/>
+    <mergeCell ref="A322:B322"/>
+    <mergeCell ref="A323:B323"/>
+    <mergeCell ref="A324:B324"/>
+    <mergeCell ref="A325:B325"/>
+    <mergeCell ref="A326:B326"/>
+    <mergeCell ref="H312:K312"/>
+    <mergeCell ref="H313:K313"/>
+    <mergeCell ref="H314:K314"/>
+    <mergeCell ref="H315:K315"/>
+    <mergeCell ref="H316:K316"/>
+    <mergeCell ref="H317:K317"/>
+    <mergeCell ref="H318:K318"/>
+    <mergeCell ref="H319:K319"/>
+    <mergeCell ref="H320:K320"/>
+    <mergeCell ref="H303:K303"/>
+    <mergeCell ref="H304:K304"/>
+    <mergeCell ref="H305:K305"/>
+    <mergeCell ref="H306:K306"/>
+    <mergeCell ref="H307:K307"/>
+    <mergeCell ref="H308:K308"/>
+    <mergeCell ref="H309:K309"/>
+    <mergeCell ref="H310:K310"/>
+    <mergeCell ref="H311:K311"/>
+    <mergeCell ref="H325:K325"/>
+    <mergeCell ref="H326:K326"/>
+    <mergeCell ref="H327:K327"/>
+    <mergeCell ref="H328:K328"/>
+    <mergeCell ref="H329:K329"/>
+    <mergeCell ref="H330:K330"/>
+    <mergeCell ref="H331:K331"/>
+    <mergeCell ref="H332:K332"/>
+    <mergeCell ref="A332:B332"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>